<commit_message>
SBV UE02 Korrekturen Anfang
</commit_message>
<xml_diff>
--- a/FH/Tutorium/SBV/UE_1b/SBV_UE01B.xlsx
+++ b/FH/Tutorium/SBV/UE_1b/SBV_UE01B.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Git\Development\FH\Tutorium\SBV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FH\Tutorium\SBV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3DBF3D5-E7AF-4500-89A2-82F3129CE75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F931E592-688E-495A-85F6-C1F54B4A5764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2490" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{933D98FB-FEB6-4BBF-84D7-D88FDCEFBD74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12336" activeTab="1" xr2:uid="{933D98FB-FEB6-4BBF-84D7-D88FDCEFBD74}"/>
   </bookViews>
   <sheets>
     <sheet name="1a" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>Julian Buchgeher</t>
   </si>
@@ -157,35 +157,37 @@
     <t>Sehr gut dokumentiert!</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Nur kurz erklärt + richtig für in Bewegung?</t>
-  </si>
-  <si>
     <t>Korrekturen echt aufwändig und super!</t>
   </si>
   <si>
-    <t>Schaut gut aus</t>
-  </si>
-  <si>
     <t>[-1] Monotones Bild (einfarbig) als guess nicht getestet?</t>
   </si>
   <si>
-    <t>c etwas wenig?</t>
-  </si>
-  <si>
-    <t>Anderes Bild: Was wurde verwendet?</t>
-  </si>
-  <si>
     <t>[-1] Es existieren mehrere lokale Maxima rund um den Mittelpunkt: Warum nur einer entfernt bzw. asymmetrisch? Allgemein etwas wenig beschrieben.</t>
   </si>
   <si>
-    <t>Mega ausführlich beschrieben, Analyse eher unübersichtlich?</t>
-  </si>
-  <si>
-    <t>[-1] Nur mit einem Bild getestet. Dadurch zeigt sich auch das Problem mit Nulldivision nicht (würde höchstwahrscheinlich bei anderen Bildern auffallen)
+    <t>[-1] Nur mit einem Bild getestet. 
 [-0.5] Nur Division durch 0 verhindert. Es können sich aber Werte &gt; 255 ergeben, die zu Artefakten/Overflows führen.</t>
+  </si>
+  <si>
+    <t>Sehr gut!</t>
+  </si>
+  <si>
+    <t>[-0.25] Anderes Bild: Was wurde verwendet?</t>
+  </si>
+  <si>
+    <t>[-1.5] Bei der HRV sind eigentlich nur die RR-Intervalle relevant, und nicht die Abstände zwischen allen Maxima/Minima und diese hier sinnvoll abzulesen ist schwierig.</t>
+  </si>
+  <si>
+    <t>Sehr ausführliche und gute Analyse!
+[-1.5] Die Antwort hier ist recht grob, bzw. großteils Antwort auf Teil a). Die HRV sollte wirklich genauer hergeleitet oder geplottet werden (z.B. RMSSD, bei ruhigem RESP)
+Es tut mir Leid, dass ihr hier so viel Aufwand hattet. Ein Teil ergibt sich wahrscheinlich dadurch, dass ihr nicht nur RESP, sondern auch EDA analysiert habt. Werde das Feedback  auch so weitergeben.</t>
+  </si>
+  <si>
+    <t>[-1.5] HRV sollte näher bzw. geplotted berechnet werden (z.B. RMSSD bei ruhigem RMSSD). Analyse für "Mit Bewegung" allgemein recht mager.</t>
+  </si>
+  <si>
+    <t>[-3] Hier wird nicht auf b) aufgebaut bzw. nichts berechnet/gezeigt/vermutet. Hier wäre verlangt gewesen, wirklich zu analysieren wie hoch die HRV in den Messungen ist.</t>
   </si>
 </sst>
 </file>
@@ -288,6 +290,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,9 +301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,75 +618,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216AA612-AD3A-47AA-A21E-B3AB36ED0108}">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView topLeftCell="G7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="3"/>
-    <col min="3" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2"/>
-    <col min="7" max="7" width="19.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="10"/>
-    <col min="9" max="10" width="8.85546875" style="11"/>
-    <col min="11" max="11" width="19.7109375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="3"/>
-    <col min="13" max="14" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="19.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="10"/>
+    <col min="9" max="10" width="8.88671875" style="11"/>
+    <col min="11" max="11" width="19.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="3"/>
+    <col min="13" max="14" width="8.88671875" style="2"/>
     <col min="15" max="15" width="20" style="4" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="10"/>
-    <col min="17" max="20" width="8.85546875" style="11"/>
+    <col min="16" max="16" width="8.88671875" style="10"/>
+    <col min="17" max="20" width="8.88671875" style="11"/>
     <col min="21" max="21" width="22" style="12" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="2"/>
-    <col min="25" max="25" width="12.85546875" style="4" customWidth="1"/>
-    <col min="29" max="29" width="18.85546875" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" style="2"/>
+    <col min="25" max="25" width="12.88671875" style="4" customWidth="1"/>
+    <col min="29" max="29" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="13">
+      <c r="B1" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="14">
+      <c r="H1" s="15">
         <v>1.2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16">
         <v>1.3</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="14">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="15">
         <v>1.4</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="15">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="16">
         <v>1.5</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -770,7 +772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="210.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="173.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -849,7 +851,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -936,7 +938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="210" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>0.92307692307692313</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -1190,7 +1192,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>0.88235294117647056</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="210" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1659,7 +1661,7 @@
         <v>0.92307692307692313</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="285" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="210" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1840,7 +1842,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="1" customFormat="1" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" s="1" customFormat="1" ht="259.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -2002,53 +2004,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685DA3C3-B6A0-4A2F-BAD5-0A5D2E51AD69}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" customWidth="1"/>
-    <col min="17" max="17" width="30.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.28515625" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="25.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.88671875" customWidth="1"/>
+    <col min="12" max="16" width="8.88671875" style="2"/>
+    <col min="17" max="17" width="30.5546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.33203125" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B1" s="2">
         <v>1.5</v>
       </c>
       <c r="F1">
         <v>1.6</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="2">
         <v>1.7</v>
       </c>
       <c r="R1">
         <v>1.8</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
@@ -2069,22 +2073,22 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R2" t="s">
@@ -2105,108 +2109,108 @@
       <c r="W2" t="s">
         <v>16</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16">
-        <v>4</v>
-      </c>
-      <c r="C3" s="16">
-        <v>4</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
         <f>SUM(B3)</f>
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>8</v>
       </c>
-      <c r="G3" s="16">
-        <v>3</v>
-      </c>
-      <c r="H3" s="16">
-        <v>2</v>
-      </c>
-      <c r="I3" s="16">
+      <c r="G3" s="13">
+        <v>3</v>
+      </c>
+      <c r="H3" s="13">
+        <v>2</v>
+      </c>
+      <c r="I3" s="13">
         <v>13</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="13">
         <f>F3+G3+H3</f>
         <v>13</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>6.5</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="16">
-        <v>12</v>
-      </c>
-      <c r="P3" s="16" t="e">
+      <c r="K3" s="13"/>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>7</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O3" s="4">
+        <v>12</v>
+      </c>
+      <c r="P3" s="4">
         <f>L3+M3+N3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16">
-        <v>0</v>
-      </c>
-      <c r="V3" s="16">
+        <v>10.5</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13">
+        <v>0</v>
+      </c>
+      <c r="V3" s="13">
         <f>R3+S3+T3</f>
         <v>0</v>
       </c>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16">
+      <c r="W3" s="13"/>
+      <c r="X3" s="4">
         <f>U3+O3+I3+C3</f>
         <v>29</v>
       </c>
-      <c r="Y3" s="16" t="e">
+      <c r="Y3" s="4">
         <f>V3+P3+J3+D3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z3" s="16" t="e">
-        <f>X3/Y3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA3" s="16"/>
+        <v>27.5</v>
+      </c>
+      <c r="Z3" s="4">
+        <f>Y3/X3</f>
+        <v>0.94827586206896552</v>
+      </c>
+      <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
         <f t="shared" ref="D4:D15" si="0">SUM(B4)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <v>8</v>
       </c>
       <c r="G4">
@@ -2215,746 +2219,1099 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="13">
         <v>13</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="13">
         <f t="shared" ref="J4:J15" si="1">F4+G4+H4</f>
         <v>13</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="16">
-        <v>12</v>
-      </c>
-      <c r="P4" s="16" t="e">
+      <c r="K4" s="13"/>
+      <c r="L4" s="4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>7</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="4">
+        <v>12</v>
+      </c>
+      <c r="P4" s="4">
         <f t="shared" ref="P4:P15" si="2">L4+M4+N4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" s="16">
+        <v>10.5</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="13">
         <v>10</v>
       </c>
-      <c r="S4" s="16">
-        <v>3</v>
-      </c>
-      <c r="T4" s="16">
-        <v>3</v>
-      </c>
-      <c r="U4" s="16">
+      <c r="S4" s="13">
+        <v>3</v>
+      </c>
+      <c r="T4" s="13">
+        <v>3</v>
+      </c>
+      <c r="U4" s="13">
         <v>16</v>
       </c>
-      <c r="V4" s="16">
+      <c r="V4" s="13">
         <f t="shared" ref="V4:V16" si="3">R4+S4+T4</f>
         <v>16</v>
       </c>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16">
+      <c r="W4" s="13"/>
+      <c r="X4" s="4">
         <f t="shared" ref="X4:Y15" si="4">U4+O4+I4+C4</f>
         <v>41</v>
       </c>
-      <c r="Y4" s="16" t="e">
+      <c r="Y4" s="4">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z4" s="16" t="e">
-        <f t="shared" ref="Z4:Z15" si="5">X4/Y4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA4" s="16"/>
+        <v>39.5</v>
+      </c>
+      <c r="Z4" s="4">
+        <f t="shared" ref="Z4:Z16" si="5">Y4/X4</f>
+        <v>0.96341463414634143</v>
+      </c>
+      <c r="AA4" s="13"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16">
+      <c r="B5" s="4">
+        <f>B3</f>
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:Z5" si="6">C3</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>Sehr gut dokumentiert!</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="6"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q5" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>[-1.5] HRV sollte näher bzw. geplotted berechnet werden (z.B. RMSSD bei ruhigem RMSSD). Analyse für "Mit Bewegung" allgemein recht mager.</v>
+      </c>
+      <c r="R5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+      <c r="Y5" s="4">
+        <f t="shared" si="6"/>
+        <v>27.5</v>
+      </c>
+      <c r="Z5" s="4">
+        <f t="shared" si="5"/>
+        <v>0.94827586206896552</v>
+      </c>
+      <c r="AA5" s="13"/>
+    </row>
+    <row r="6" spans="1:27" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="13">
+        <v>8</v>
+      </c>
+      <c r="G6" s="13">
+        <v>3</v>
+      </c>
+      <c r="I6" s="13">
+        <v>11</v>
+      </c>
+      <c r="J6" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16">
+        <v>11</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>7</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>12</v>
+      </c>
+      <c r="P6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="13">
+        <v>10</v>
+      </c>
+      <c r="S6" s="13">
+        <v>2.75</v>
+      </c>
+      <c r="T6" s="13">
+        <v>3</v>
+      </c>
+      <c r="U6" s="13">
+        <v>16</v>
+      </c>
+      <c r="V6" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16">
+        <v>15.75</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="4">
+        <f>U6+O6+I6+C6</f>
+        <v>43</v>
+      </c>
+      <c r="Y6" s="4">
+        <f>V6+P6+J6+D6</f>
+        <v>39.75</v>
+      </c>
+      <c r="Z6" s="4">
+        <f t="shared" si="5"/>
+        <v>0.92441860465116277</v>
+      </c>
+      <c r="AA6" s="13"/>
+    </row>
+    <row r="7" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="13">
+        <v>8</v>
+      </c>
+      <c r="G7" s="13">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="13">
+        <v>13</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>7</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>12</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" s="13">
+        <v>10</v>
+      </c>
+      <c r="S7" s="13">
+        <v>2</v>
+      </c>
+      <c r="T7" s="13">
+        <v>3</v>
+      </c>
+      <c r="U7" s="13">
+        <v>16</v>
+      </c>
+      <c r="V7" s="13">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="W7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="16">
+        <v>45</v>
+      </c>
+      <c r="Y7" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="16" t="e">
+        <v>44</v>
+      </c>
+      <c r="Z7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="AA7" s="13"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="13"/>
+      <c r="X8" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA5" s="16"/>
+      <c r="AA8" s="13"/>
     </row>
-    <row r="6" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="16">
-        <v>4</v>
-      </c>
-      <c r="C6" s="16">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16">
+    <row r="9" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B7</f>
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:Z9" si="7">C7</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>Korrekturen echt aufwändig und super!</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="Q9" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>Sehr gut!</v>
+      </c>
+      <c r="R9" s="13">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="T9" s="13">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="U9" s="13">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="V9" s="13">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="W9" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>[-1] Monotones Bild (einfarbig) als guess nicht getestet?</v>
+      </c>
+      <c r="X9" s="4">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="Y9" s="4">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="Z9" s="4">
+        <f t="shared" si="5"/>
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="AA9" s="13"/>
+    </row>
+    <row r="10" spans="1:27" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B4</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" ref="C10:Z10" si="8">C4</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1a</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="8"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q10" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>[-1.5] Bei der HRV sind eigentlich nur die RR-Intervalle relevant, und nicht die Abstände zwischen allen Maxima/Minima und diese hier sinnvoll abzulesen ist schwierig.</v>
+      </c>
+      <c r="R10" s="13">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="S10" s="13">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="T10" s="13">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="U10" s="13">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="V10" s="13">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="W10" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="Y10" s="4">
+        <f t="shared" si="8"/>
+        <v>39.5</v>
+      </c>
+      <c r="Z10" s="4">
+        <f t="shared" si="5"/>
+        <v>0.96341463414634143</v>
+      </c>
+      <c r="AA10" s="13"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="13"/>
+      <c r="X11" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA11" s="13"/>
+    </row>
+    <row r="12" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B6</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:Z12" si="9">C6</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="G6" s="16">
-        <v>3</v>
-      </c>
-      <c r="I6" s="16">
+      <c r="G12" s="13">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J12" s="13">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="Q12" s="4" t="str">
+        <f>Q6</f>
+        <v>[-3] Hier wird nicht auf b) aufgebaut bzw. nichts berechnet/gezeigt/vermutet. Hier wäre verlangt gewesen, wirklich zu analysieren wie hoch die HRV in den Messungen ist.</v>
+      </c>
+      <c r="R12" s="13">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="S12" s="13">
+        <f t="shared" si="9"/>
+        <v>2.75</v>
+      </c>
+      <c r="T12" s="13">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="U12" s="13">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="V12" s="13">
+        <f t="shared" si="9"/>
+        <v>15.75</v>
+      </c>
+      <c r="W12" s="13" t="str">
+        <f>W6</f>
+        <v>[-0.25] Anderes Bild: Was wurde verwendet?</v>
+      </c>
+      <c r="X12" s="4">
+        <f t="shared" si="9"/>
+        <v>43</v>
+      </c>
+      <c r="Y12" s="4">
+        <f t="shared" si="9"/>
+        <v>39.75</v>
+      </c>
+      <c r="Z12" s="4">
+        <f t="shared" si="5"/>
+        <v>0.92441860465116277</v>
+      </c>
+      <c r="AA12" s="13"/>
+    </row>
+    <row r="13" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13" s="13">
+        <v>13</v>
+      </c>
+      <c r="J13" s="13">
         <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="4">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>7</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O13" s="4">
+        <v>12</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R13" s="13">
+        <v>10</v>
+      </c>
+      <c r="S13" s="13">
+        <v>2</v>
+      </c>
+      <c r="T13" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="U13" s="13">
+        <v>16</v>
+      </c>
+      <c r="V13" s="13">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+      <c r="W13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="Y13" s="4">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="Z13" s="4">
+        <f t="shared" si="5"/>
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="AA13" s="13"/>
+    </row>
+    <row r="14" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4">
+        <f>B3</f>
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" ref="C14:Z14" si="10">C3</f>
+        <v>4</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Sehr gut dokumentiert!</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="10"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q14" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>[-1.5] HRV sollte näher bzw. geplotted berechnet werden (z.B. RMSSD bei ruhigem RMSSD). Analyse für "Mit Bewegung" allgemein recht mager.</v>
+      </c>
+      <c r="R14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="10"/>
+        <v>29</v>
+      </c>
+      <c r="Y14" s="4">
+        <f t="shared" si="10"/>
+        <v>27.5</v>
+      </c>
+      <c r="Z14" s="4">
+        <f t="shared" si="5"/>
+        <v>0.94827586206896552</v>
+      </c>
+      <c r="AA14" s="13"/>
+    </row>
+    <row r="15" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16">
-        <v>2</v>
-      </c>
-      <c r="M6">
+      <c r="B15" s="4">
+        <f>B13</f>
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ref="C15:Z16" si="11">C13</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f>E13</f>
+        <v>[-1] Es existieren mehrere lokale Maxima rund um den Mittelpunkt: Warum nur einer entfernt bzw. asymmetrisch? Allgemein etwas wenig beschrieben.</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="J15" s="13">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="16">
-        <v>12</v>
-      </c>
-      <c r="P6" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16">
+      <c r="N15" s="4">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="11"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q15" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>Sehr ausführliche und gute Analyse!
+[-1.5] Die Antwort hier ist recht grob, bzw. großteils Antwort auf Teil a). Die HRV sollte wirklich genauer hergeleitet oder geplottet werden (z.B. RMSSD, bei ruhigem RESP)
+Es tut mir Leid, dass ihr hier so viel Aufwand hattet. Ein Teil ergibt sich wahrscheinlich dadurch, dass ihr nicht nur RESP, sondern auch EDA analysiert habt. Werde das Feedback  auch so weitergeben.</v>
+      </c>
+      <c r="R15" s="13">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="S6" s="16">
-        <v>3</v>
-      </c>
-      <c r="T6" s="16">
-        <v>3</v>
-      </c>
-      <c r="U6" s="16">
+      <c r="S15" s="13">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="T15" s="13">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="U15" s="13">
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="V6" s="16">
+      <c r="V15" s="13">
+        <f t="shared" si="11"/>
+        <v>14.5</v>
+      </c>
+      <c r="W15" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>[-1] Nur mit einem Bild getestet. 
+[-0.5] Nur Division durch 0 verhindert. Es können sich aber Werte &gt; 255 ergeben, die zu Artefakten/Overflows führen.</v>
+      </c>
+      <c r="X15" s="4">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="Y15" s="4">
+        <f t="shared" si="11"/>
+        <v>41</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" si="5"/>
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="AA15" s="13"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>13</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>7</v>
+      </c>
+      <c r="N16" s="2">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+      <c r="U16">
+        <v>16</v>
+      </c>
+      <c r="V16" s="13">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="W6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="X6" s="16">
-        <f>U6+O6+I6+C6</f>
-        <v>43</v>
-      </c>
-      <c r="Y6" s="16" t="e">
-        <f>V6+P6+J6+D6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z6" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA6" s="16"/>
-    </row>
-    <row r="7" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="16">
-        <v>4</v>
-      </c>
-      <c r="C7" s="16">
-        <v>4</v>
-      </c>
-      <c r="D7" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="16">
-        <v>8</v>
-      </c>
-      <c r="G7" s="16">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="16">
-        <v>13</v>
-      </c>
-      <c r="J7" s="16" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>7</v>
-      </c>
-      <c r="N7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="16">
-        <v>12</v>
-      </c>
-      <c r="P7" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" s="16">
-        <v>10</v>
-      </c>
-      <c r="S7" s="16">
-        <v>2</v>
-      </c>
-      <c r="T7" s="16">
-        <v>3</v>
-      </c>
-      <c r="U7" s="16">
-        <v>16</v>
-      </c>
-      <c r="V7" s="16">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="W7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="X7" s="16">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="Y7" s="16" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z7" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA7" s="16"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA8" s="16"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA9" s="16"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y10" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA10" s="16"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA11" s="16"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA12" s="16"/>
-    </row>
-    <row r="13" spans="1:27" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="16">
-        <v>3</v>
-      </c>
-      <c r="C13" s="16">
-        <v>4</v>
-      </c>
-      <c r="D13" s="16">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="16">
-        <v>8</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13" s="16">
-        <v>13</v>
-      </c>
-      <c r="J13" s="16">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16">
-        <v>2</v>
-      </c>
-      <c r="M13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" s="16">
-        <v>12</v>
-      </c>
-      <c r="P13" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="R13" s="16">
-        <v>10</v>
-      </c>
-      <c r="S13" s="16">
-        <v>2</v>
-      </c>
-      <c r="T13" s="16">
-        <v>2.5</v>
-      </c>
-      <c r="U13" s="16">
-        <v>16</v>
-      </c>
-      <c r="V13" s="16">
-        <f t="shared" si="3"/>
-        <v>14.5</v>
-      </c>
-      <c r="W13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="X13" s="16">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="Y13" s="16" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z13" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA13" s="16"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X14" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA14" s="16"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA15" s="16"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>8</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>13</v>
-      </c>
-      <c r="L16">
-        <v>2</v>
-      </c>
-      <c r="M16">
-        <v>7</v>
-      </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
-      <c r="R16">
-        <v>10</v>
-      </c>
-      <c r="S16">
-        <v>3</v>
-      </c>
-      <c r="T16">
-        <v>3</v>
-      </c>
-      <c r="U16">
-        <v>16</v>
-      </c>
-      <c r="V16" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>